<commit_message>
clean copies of attachments
</commit_message>
<xml_diff>
--- a/scirep/Copy of WP_and_Mortality for week7_7_2015.xlsx
+++ b/scirep/Copy of WP_and_Mortality for week7_7_2015.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24426"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="620" yWindow="2160" windowWidth="23000" windowHeight="15320"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -92,15 +92,6 @@
   </si>
   <si>
     <t>R2SC1-RR-1</t>
-  </si>
-  <si>
-    <t>Rachel's notes</t>
-  </si>
-  <si>
-    <t>disease present Nov 12 2014</t>
-  </si>
-  <si>
-    <t>Coral 10 does not appear in the photo list</t>
   </si>
 </sst>
 </file>
@@ -161,9 +152,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J23" totalsRowShown="0">
-  <autoFilter ref="A1:J23"/>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I23" totalsRowShown="0">
+  <autoFilter ref="A1:I23"/>
+  <tableColumns count="9">
     <tableColumn id="1" name="Date" dataDxfId="0"/>
     <tableColumn id="2" name="Week Number"/>
     <tableColumn id="3" name="visit"/>
@@ -173,7 +164,6 @@
     <tableColumn id="7" name="Coral ID"/>
     <tableColumn id="8" name="Condition code QA/QC (0-1)"/>
     <tableColumn id="9" name="Condition QA/QC"/>
-    <tableColumn id="10" name="Rachel's notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -466,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -483,7 +473,7 @@
     <col min="9" max="9" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -511,11 +501,8 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>42192</v>
       </c>
@@ -537,11 +524,8 @@
       <c r="I2" t="s">
         <v>12</v>
       </c>
-      <c r="J2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>42192</v>
       </c>
@@ -563,11 +547,8 @@
       <c r="I3" t="s">
         <v>12</v>
       </c>
-      <c r="J3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>42192</v>
       </c>
@@ -590,7 +571,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>42192</v>
       </c>
@@ -613,7 +594,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:9">
       <c r="A6" s="1">
         <v>42192</v>
       </c>
@@ -636,7 +617,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:9">
       <c r="A7" s="1">
         <v>42192</v>
       </c>
@@ -659,7 +640,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:9">
       <c r="A8" s="1">
         <v>42192</v>
       </c>
@@ -682,7 +663,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:9">
       <c r="A9" s="1">
         <v>42192</v>
       </c>
@@ -705,7 +686,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:9">
       <c r="A10" s="1">
         <v>42192</v>
       </c>
@@ -728,7 +709,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:9">
       <c r="A11" s="1">
         <v>42192</v>
       </c>
@@ -751,7 +732,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:9">
       <c r="A12" s="1">
         <v>42192</v>
       </c>
@@ -774,7 +755,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:9">
       <c r="A13" s="1">
         <v>42192</v>
       </c>
@@ -797,7 +778,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:9">
       <c r="A14" s="1">
         <v>42192</v>
       </c>
@@ -820,7 +801,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:9">
       <c r="A15" s="1">
         <v>42192</v>
       </c>
@@ -843,7 +824,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:9">
       <c r="A16" s="1">
         <v>42192</v>
       </c>

</xml_diff>